<commit_message>
Add some other obs from 2022
</commit_message>
<xml_diff>
--- a/data/raw/Dieren en Planten Waarnemingen from 2022-01-01.xlsx
+++ b/data/raw/Dieren en Planten Waarnemingen from 2022-01-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damiano_oldoni\Documents\GitHub\vmm-rattenapp-occurrences\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD54FD3-C98A-410C-B135-2D5F3DAF9B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92B4121-2C24-4051-AA3D-CD30ACC113E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="81">
   <si>
     <t>Jaar</t>
   </si>
@@ -180,6 +180,90 @@
   </si>
   <si>
     <t>Dendermonde</t>
+  </si>
+  <si>
+    <t>MAAS LIMBURG</t>
+  </si>
+  <si>
+    <t>Denderbekken</t>
+  </si>
+  <si>
+    <t>Aalst</t>
+  </si>
+  <si>
+    <t>Vuilzakken</t>
+  </si>
+  <si>
+    <t>Spiere-Helkijn</t>
+  </si>
+  <si>
+    <t>DIJLE EN ZENNE</t>
+  </si>
+  <si>
+    <t>Dijle- en Zennebekken</t>
+  </si>
+  <si>
+    <t>KANAAL LEUVEN-DIJLE - KANAAL VAN LEUVEN NAAR DE DIJLE</t>
+  </si>
+  <si>
+    <t>Vlaams-Brabant</t>
+  </si>
+  <si>
+    <t>Kampenhout</t>
+  </si>
+  <si>
+    <t>Grote waternavel</t>
+  </si>
+  <si>
+    <t>ANB-Waterplanten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waargenomen        </t>
+  </si>
+  <si>
+    <t>Polder of wateringgracht</t>
+  </si>
+  <si>
+    <t>Knokke-Heist</t>
+  </si>
+  <si>
+    <t>DEMER</t>
+  </si>
+  <si>
+    <t>Demerbekken</t>
+  </si>
+  <si>
+    <t>ZUTENDAALBEEK</t>
+  </si>
+  <si>
+    <t>Limburg</t>
+  </si>
+  <si>
+    <t>Zutendaal</t>
+  </si>
+  <si>
+    <t>ISABELLAVAART - KLEINE GEULE</t>
+  </si>
+  <si>
+    <t>Woelrat</t>
+  </si>
+  <si>
+    <t>RIJTGRACHT - PACHTBEEK - OLIEBERGBEEK</t>
+  </si>
+  <si>
+    <t>Avelgem</t>
+  </si>
+  <si>
+    <t>Natuurgebied</t>
+  </si>
+  <si>
+    <t>Leiebekken</t>
+  </si>
+  <si>
+    <t>TOLBEEK</t>
+  </si>
+  <si>
+    <t>Wevelgem</t>
   </si>
 </sst>
 </file>
@@ -613,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:S2491"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J3" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1283,256 +1367,702 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4">
+        <v>44571</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" s="5">
+        <v>137299</v>
+      </c>
+      <c r="M15" s="6">
+        <v>4.0444033023359198</v>
+      </c>
+      <c r="N15" s="6">
+        <v>50.944339968671798</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P15" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R15" s="5">
+        <v>535509</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="4">
+        <v>44571</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L16" s="5">
+        <v>137309</v>
+      </c>
+      <c r="M16" s="6">
+        <v>4.0444710281176102</v>
+      </c>
+      <c r="N16" s="6">
+        <v>50.944348015299298</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P16" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R16" s="5">
+        <v>535525</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="4">
+        <v>44571</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="5">
+        <v>137338</v>
+      </c>
+      <c r="M17" s="6">
+        <v>3.3398925641114898</v>
+      </c>
+      <c r="N17" s="6">
+        <v>50.73213179303</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P17" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R17" s="5">
+        <v>535572</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="A18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="4">
+        <v>44571</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="5">
+        <v>137398</v>
+      </c>
+      <c r="M18" s="6">
+        <v>4.0444626462139297</v>
+      </c>
+      <c r="N18" s="6">
+        <v>50.944299064981898</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P18" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R18" s="5">
+        <v>535662</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="4">
+        <v>44572</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" s="5">
+        <v>137471</v>
+      </c>
+      <c r="M19" s="6">
+        <v>3.58982886164361</v>
+      </c>
+      <c r="N19" s="6">
+        <v>51.260769908027001</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P19" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R19" s="5">
+        <v>535878</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="3"/>
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="4">
+        <v>44573</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L20" s="5">
+        <v>137607</v>
+      </c>
+      <c r="M20" s="6">
+        <v>4.6049863609663397</v>
+      </c>
+      <c r="N20" s="6">
+        <v>50.954578464006097</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P20" s="4">
+        <v>43801</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>44727</v>
+      </c>
+      <c r="R20" s="5">
+        <v>536201</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="4">
+        <v>44573</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L21" s="5">
+        <v>137691</v>
+      </c>
+      <c r="M21" s="6">
+        <v>3.3678554329488</v>
+      </c>
+      <c r="N21" s="6">
+        <v>51.334779099957899</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R21" s="5">
+        <v>536372</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="3"/>
+      <c r="A22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="4">
+        <v>44573</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L22" s="5">
+        <v>137759</v>
+      </c>
+      <c r="M22" s="6">
+        <v>5.5332117845542301</v>
+      </c>
+      <c r="N22" s="6">
+        <v>50.908417141194199</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P22" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R22" s="5">
+        <v>536538</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="3"/>
+      <c r="A23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4">
+        <v>44575</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L23" s="5">
+        <v>137963</v>
+      </c>
+      <c r="M23" s="6">
+        <v>3.3684540685089801</v>
+      </c>
+      <c r="N23" s="6">
+        <v>51.335805883157597</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P23" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R23" s="5">
+        <v>536884</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="3"/>
+      <c r="A24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="4">
+        <v>44575</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="5">
+        <v>138035</v>
+      </c>
+      <c r="M24" s="6">
+        <v>3.4821835931946898</v>
+      </c>
+      <c r="N24" s="6">
+        <v>50.783272301898698</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R24" s="5">
+        <v>536986</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="3"/>
+      <c r="A25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="4">
+        <v>44579</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L25" s="5">
+        <v>138443</v>
+      </c>
+      <c r="M25" s="6">
+        <v>3.2085166176269402</v>
+      </c>
+      <c r="N25" s="6">
+        <v>50.809415627087098</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P25" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R25" s="5">
+        <v>537859</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="26" spans="1:19" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="3"/>
+      <c r="A26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="4">
+        <v>44579</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L26" s="5">
+        <v>138446</v>
+      </c>
+      <c r="M26" s="6">
+        <v>3.2083872010342702</v>
+      </c>
+      <c r="N26" s="6">
+        <v>50.809368185512298</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P26" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R26" s="5">
+        <v>537862</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="27" spans="1:19" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>

</xml_diff>

<commit_message>
Add one raw obs to test trigger workflow
</commit_message>
<xml_diff>
--- a/data/raw/Dieren en Planten Waarnemingen from 2022-01-01.xlsx
+++ b/data/raw/Dieren en Planten Waarnemingen from 2022-01-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damiano_oldoni\Documents\GitHub\vmm-rattenapp-occurrences\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDE28B0-74D9-4DB1-960A-A593534212F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923BE696-076B-4BA5-B99B-3B8A2ACFF3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2757" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2769" uniqueCount="272">
   <si>
     <t>Jaar</t>
   </si>
@@ -835,6 +835,9 @@
   <si>
     <t>Heist-op-den-Berg</t>
   </si>
+  <si>
+    <t>GELEEDBEEK - PASSENDALEGELEED - ZUIDGELEED</t>
+  </si>
 </sst>
 </file>
 
@@ -1267,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:S2491"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD236"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="A237" sqref="A237:XFD237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14949,25 +14952,63 @@
       </c>
     </row>
     <row r="237" spans="1:19" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A237" s="3"/>
-      <c r="B237" s="3"/>
-      <c r="C237" s="4"/>
-      <c r="D237" s="3"/>
-      <c r="E237" s="3"/>
-      <c r="F237" s="3"/>
-      <c r="G237" s="3"/>
-      <c r="H237" s="3"/>
-      <c r="I237" s="3"/>
-      <c r="J237" s="3"/>
-      <c r="K237" s="3"/>
-      <c r="L237" s="5"/>
-      <c r="M237" s="6"/>
-      <c r="N237" s="6"/>
-      <c r="O237" s="3"/>
-      <c r="P237" s="4"/>
-      <c r="Q237" s="4"/>
-      <c r="R237" s="5"/>
-      <c r="S237" s="3"/>
+      <c r="A237" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C237" s="4">
+        <v>44566</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F237" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G237" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="H237" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I237" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="J237" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K237" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L237" s="5">
+        <v>28635</v>
+      </c>
+      <c r="M237" s="6">
+        <v>3.0771921360309298</v>
+      </c>
+      <c r="N237" s="6">
+        <v>51.202171684185998</v>
+      </c>
+      <c r="O237" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P237" s="4">
+        <v>36526</v>
+      </c>
+      <c r="Q237" s="4">
+        <v>2958465</v>
+      </c>
+      <c r="R237" s="5">
+        <v>534379</v>
+      </c>
+      <c r="S237" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="238" spans="1:19" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A238" s="3"/>

</xml_diff>